<commit_message>
Cập nhật testcase 11/5/2015
</commit_message>
<xml_diff>
--- a/docs/testcase.xlsx
+++ b/docs/testcase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1. Đăng ký" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="4. Đăng tin" sheetId="5" r:id="rId4"/>
     <sheet name="5. Tìm kiếm và sắp xếp" sheetId="6" r:id="rId5"/>
     <sheet name="6. Chức năng với bài đăng" sheetId="7" r:id="rId6"/>
+    <sheet name="7. Dùng khi không đăng nhập" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_b" localSheetId="4">#REF!</definedName>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="182">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -764,7 +765,45 @@
 3. Nhấn vào biểu tượng chữ i xuất hiện ở thanh công cụ phía trên bài đăng</t>
   </si>
   <si>
-    <t>Hiển thị thông tin bao gồm: thông tin bài đăng (hình ảnh (nếu có), giá gốc, giá bán, chất lượng, mô tả) và thông tin người đăng (tên người đăng, địa chỉ, số điện thoại, email)</t>
+    <t>Dùng khi không đăng nhập</t>
+  </si>
+  <si>
+    <t>Không đăng nhập, đăng kí tài khoản</t>
+  </si>
+  <si>
+    <t>1. Vào giao diện chính
+2. Chọn mục ĐĂNG TIN</t>
+  </si>
+  <si>
+    <t>Mở hộp đăng nhập tài khoản</t>
+  </si>
+  <si>
+    <t>Tìm kiếm sách</t>
+  </si>
+  <si>
+    <t>1. Vào giao diện chính
+2. Viết tên sách vào hộp tìm kiếm
+3. Nhấn Enter hoặc nháy vào biểu tượng tìm kiếm</t>
+  </si>
+  <si>
+    <t>Hiện thông tin bài đăng cần tìm(nếu có)</t>
+  </si>
+  <si>
+    <t>1. Vào giao diện chính
+2. Chọn biểu tượng kiểu sắp xếp muốn</t>
+  </si>
+  <si>
+    <t>Hiên thị danh sách bài đăng đã sắp xếp theo ý muốn( mặc định, theo giá, theo chất lượng)</t>
+  </si>
+  <si>
+    <t>1. Vào giao diện chính
+2. Chọn biểu tượng chữ I phía trên thanh công cụ của sách muốn xem</t>
+  </si>
+  <si>
+    <t>Chuyển sang giao diện mới là thông tin bài đăng đó: tên sách, ảnh, giá gốc, giá bán, chất lượng, mô tả, người đăng, thông tin người đăng</t>
+  </si>
+  <si>
+    <t>Hiển thị thông tin bao gồm: thông tin bài đăng (hình ảnh (nếu có), giá gốc, giá bán(đã tính độ giảm so với giá gốc), chất lượng, mô tả) và thông tin người đăng (tên người đăng, địa chỉ, số điện thoại, email)</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1138,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1379,6 +1418,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1419,6 +1467,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1697,7 +1748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1727,10 +1778,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="95"/>
+      <c r="E1" s="98"/>
       <c r="F1" s="1"/>
       <c r="G1" s="50"/>
       <c r="H1" s="2"/>
@@ -1740,10 +1791,10 @@
       <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="96"/>
+      <c r="C2" s="99"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
@@ -1755,10 +1806,10 @@
       <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="6"/>
@@ -1770,10 +1821,10 @@
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="102">
         <v>13</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="6"/>
@@ -2276,10 +2327,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2289,10 +2340,10 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="96"/>
+      <c r="C2" s="99"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
@@ -2304,10 +2355,10 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="6"/>
@@ -2319,11 +2370,11 @@
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="102">
         <f>COUNTA(A7:A99)</f>
         <v>6</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="6"/>
@@ -2602,10 +2653,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2615,10 +2666,10 @@
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="98"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="41"/>
@@ -2647,10 +2698,10 @@
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="41"/>
@@ -2679,11 +2730,11 @@
       <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="104">
+      <c r="B4" s="107">
         <f>COUNTA(A7:A100)</f>
         <v>11</v>
       </c>
-      <c r="C4" s="105"/>
+      <c r="C4" s="108"/>
       <c r="D4" s="42"/>
       <c r="E4" s="42"/>
       <c r="F4" s="41"/>
@@ -3011,7 +3062,7 @@
       <c r="E12" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="101" t="s">
+      <c r="F12" s="104" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="83">
@@ -3020,7 +3071,7 @@
       <c r="H12" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="102" t="s">
+      <c r="I12" s="105" t="s">
         <v>101</v>
       </c>
       <c r="J12" s="21"/>
@@ -3056,14 +3107,14 @@
       <c r="E13" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="101"/>
+      <c r="F13" s="104"/>
       <c r="G13" s="83">
         <v>42130</v>
       </c>
       <c r="H13" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="102"/>
+      <c r="I13" s="105"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
@@ -3097,14 +3148,14 @@
       <c r="E14" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="101"/>
+      <c r="F14" s="104"/>
       <c r="G14" s="83">
         <v>42130</v>
       </c>
       <c r="H14" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="102"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
@@ -3138,14 +3189,14 @@
       <c r="E15" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="101"/>
+      <c r="F15" s="104"/>
       <c r="G15" s="83">
         <v>42130</v>
       </c>
       <c r="H15" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="102"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -4647,8 +4698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4671,10 +4722,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -4684,10 +4735,10 @@
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="96"/>
+      <c r="C2" s="99"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="41"/>
@@ -4716,10 +4767,10 @@
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="41"/>
@@ -4748,10 +4799,10 @@
       <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="102">
         <v>5</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="42"/>
       <c r="E4" s="42"/>
       <c r="F4" s="41"/>
@@ -4938,7 +4989,7 @@
       <c r="A9" s="70">
         <v>3</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="109" t="s">
         <v>115</v>
       </c>
       <c r="C9" s="87" t="s">
@@ -4983,7 +5034,7 @@
       <c r="A10" s="70">
         <v>4</v>
       </c>
-      <c r="B10" s="107"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="87" t="s">
         <v>110</v>
       </c>
@@ -6622,10 +6673,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -6635,10 +6686,10 @@
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="96"/>
+      <c r="C2" s="99"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="41"/>
@@ -6667,10 +6718,10 @@
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="41"/>
@@ -6699,11 +6750,11 @@
       <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="102">
         <f>COUNTA(A7:A98)</f>
         <v>7</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="42"/>
       <c r="E4" s="42"/>
       <c r="F4" s="41"/>
@@ -6804,10 +6855,10 @@
       <c r="A7" s="70">
         <v>1</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="111" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="111" t="s">
         <v>126</v>
       </c>
       <c r="D7" s="88" t="s">
@@ -6847,8 +6898,8 @@
       <c r="A8" s="70">
         <v>2</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="88" t="s">
         <v>132</v>
       </c>
@@ -6886,7 +6937,7 @@
       <c r="A9" s="70">
         <v>3</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="111" t="s">
         <v>133</v>
       </c>
       <c r="C9" s="87" t="s">
@@ -6929,7 +6980,7 @@
       <c r="A10" s="70">
         <v>4</v>
       </c>
-      <c r="B10" s="108"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="87" t="s">
         <v>126</v>
       </c>
@@ -6970,7 +7021,7 @@
       <c r="A11" s="70">
         <v>5</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="87" t="s">
         <v>126</v>
       </c>
@@ -7011,7 +7062,7 @@
       <c r="A12" s="70">
         <v>6</v>
       </c>
-      <c r="B12" s="108"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="87" t="s">
         <v>126</v>
       </c>
@@ -7052,7 +7103,7 @@
       <c r="A13" s="70">
         <v>7</v>
       </c>
-      <c r="B13" s="108"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="87" t="s">
         <v>126</v>
       </c>
@@ -8543,8 +8594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8563,10 +8614,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -8576,10 +8627,10 @@
       <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="96"/>
+      <c r="C2" s="99"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
@@ -8591,10 +8642,10 @@
       <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="6"/>
@@ -8606,11 +8657,11 @@
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="102">
         <f>COUNTA(A7:A99)</f>
         <v>7</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="6"/>
@@ -8834,7 +8885,7 @@
         <v>169</v>
       </c>
       <c r="E13" s="93" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F13" s="82" t="s">
         <v>15</v>
@@ -8864,4 +8915,1910 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="27" style="20" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="34" style="20" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="20" customWidth="1"/>
+    <col min="10" max="24" width="10.28515625" style="21" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" style="21" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="44" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="103"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" s="39" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A2" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="99"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="23"/>
+    </row>
+    <row r="3" spans="1:26" s="39" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A3" s="95" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="101"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="23"/>
+    </row>
+    <row r="4" spans="1:26" s="39" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A4" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="102">
+        <v>4</v>
+      </c>
+      <c r="C4" s="102"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="23"/>
+    </row>
+    <row r="5" spans="1:26" s="23" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+    </row>
+    <row r="6" spans="1:26" s="35" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A6" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="36"/>
+    </row>
+    <row r="7" spans="1:26" s="33" customFormat="1" ht="66.75" customHeight="1">
+      <c r="A7" s="70">
+        <v>1</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="97" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="83">
+        <v>42135</v>
+      </c>
+      <c r="H7" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="77"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+    </row>
+    <row r="8" spans="1:26" s="32" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A8" s="70">
+        <v>2</v>
+      </c>
+      <c r="B8" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="83">
+        <v>42135</v>
+      </c>
+      <c r="H8" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+    </row>
+    <row r="9" spans="1:26" s="32" customFormat="1" ht="81.75" customHeight="1">
+      <c r="A9" s="70">
+        <v>3</v>
+      </c>
+      <c r="B9" s="112" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="83">
+        <v>42135</v>
+      </c>
+      <c r="H9" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+    </row>
+    <row r="10" spans="1:26" s="32" customFormat="1" ht="87.75" customHeight="1">
+      <c r="A10" s="70">
+        <v>4</v>
+      </c>
+      <c r="B10" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="83">
+        <v>42135</v>
+      </c>
+      <c r="H10" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="77"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+    </row>
+    <row r="11" spans="1:26" s="32" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A11" s="65"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+    </row>
+    <row r="12" spans="1:26" s="32" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+    </row>
+    <row r="13" spans="1:26" s="32" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+    </row>
+    <row r="14" spans="1:26" s="32" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+    </row>
+    <row r="15" spans="1:26" s="32" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+    </row>
+    <row r="16" spans="1:26" s="32" customFormat="1" ht="15.75">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+    </row>
+    <row r="17" spans="1:25" s="32" customFormat="1" ht="15.75">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
+    </row>
+    <row r="18" spans="1:25" s="32" customFormat="1" ht="15.75">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+    </row>
+    <row r="19" spans="1:25" s="32" customFormat="1" ht="15.75">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+    </row>
+    <row r="20" spans="1:25" ht="15.75">
+      <c r="A20" s="14"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75">
+      <c r="A21" s="14"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75">
+      <c r="A22" s="14"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75">
+      <c r="A23" s="14"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75">
+      <c r="A24" s="14"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75">
+      <c r="A25" s="14"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75">
+      <c r="A26" s="14"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.75">
+      <c r="A27" s="14"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:25" ht="15.75">
+      <c r="A28" s="14"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="1:25" ht="15.75">
+      <c r="A29" s="14"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="27"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75">
+      <c r="A30" s="14"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="27"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.75">
+      <c r="A31" s="14"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="1:25" ht="15.75">
+      <c r="A32" s="14"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+    </row>
+    <row r="33" spans="1:25" ht="15.75">
+      <c r="A33" s="14"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+    </row>
+    <row r="34" spans="1:25" ht="15.75">
+      <c r="A34" s="14"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
+      <c r="Y34" s="20"/>
+    </row>
+    <row r="35" spans="1:25" ht="15.75">
+      <c r="A35" s="14"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+    </row>
+    <row r="36" spans="1:25" ht="15.75">
+      <c r="A36" s="14"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+    </row>
+    <row r="37" spans="1:25" ht="15.75">
+      <c r="A37" s="14"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.75">
+      <c r="A38" s="14"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+    </row>
+    <row r="39" spans="1:25" ht="15.75">
+      <c r="A39" s="14"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+    </row>
+    <row r="40" spans="1:25" ht="15.75">
+      <c r="A40" s="14"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+    </row>
+    <row r="41" spans="1:25" ht="15.75">
+      <c r="A41" s="14"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="20"/>
+      <c r="W41" s="20"/>
+      <c r="X41" s="20"/>
+      <c r="Y41" s="20"/>
+    </row>
+    <row r="42" spans="1:25" ht="15.75">
+      <c r="A42" s="14"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+    </row>
+    <row r="43" spans="1:25" ht="15.75">
+      <c r="A43" s="14"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+    </row>
+    <row r="44" spans="1:25" ht="15.75">
+      <c r="A44" s="14"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+    </row>
+    <row r="45" spans="1:25" ht="15.75">
+      <c r="A45" s="14"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+    </row>
+    <row r="46" spans="1:25" ht="15.75">
+      <c r="A46" s="14"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="20"/>
+      <c r="T46" s="20"/>
+      <c r="U46" s="20"/>
+      <c r="V46" s="20"/>
+      <c r="W46" s="20"/>
+      <c r="X46" s="20"/>
+      <c r="Y46" s="20"/>
+    </row>
+    <row r="47" spans="1:25" ht="15.75">
+      <c r="A47" s="14"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="20"/>
+      <c r="X47" s="20"/>
+      <c r="Y47" s="20"/>
+    </row>
+    <row r="48" spans="1:25" ht="15.75">
+      <c r="A48" s="14"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+    </row>
+    <row r="49" spans="1:25" ht="15.75">
+      <c r="A49" s="14"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+    </row>
+    <row r="50" spans="1:25" ht="15.75">
+      <c r="A50" s="14"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="20"/>
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
+    </row>
+    <row r="51" spans="1:25" ht="15.75">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="20"/>
+      <c r="T51" s="20"/>
+      <c r="U51" s="20"/>
+      <c r="V51" s="20"/>
+      <c r="W51" s="20"/>
+      <c r="X51" s="20"/>
+      <c r="Y51" s="20"/>
+    </row>
+    <row r="52" spans="1:25" ht="15.75">
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="20"/>
+      <c r="S52" s="20"/>
+      <c r="T52" s="20"/>
+      <c r="U52" s="20"/>
+      <c r="V52" s="20"/>
+      <c r="W52" s="20"/>
+      <c r="X52" s="20"/>
+      <c r="Y52" s="20"/>
+    </row>
+    <row r="53" spans="1:25" ht="15.75">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="20"/>
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="20"/>
+      <c r="X53" s="20"/>
+      <c r="Y53" s="20"/>
+    </row>
+    <row r="54" spans="1:25" ht="15.75">
+      <c r="A54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="20"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+    </row>
+    <row r="55" spans="1:25" ht="15.75">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="20"/>
+      <c r="V55" s="20"/>
+      <c r="W55" s="20"/>
+      <c r="X55" s="20"/>
+      <c r="Y55" s="20"/>
+    </row>
+    <row r="56" spans="1:25" ht="15.75">
+      <c r="A56" s="14"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="20"/>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="20"/>
+      <c r="Y56" s="20"/>
+    </row>
+    <row r="57" spans="1:25" ht="15.75">
+      <c r="A57" s="14"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="20"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="20"/>
+      <c r="T57" s="20"/>
+      <c r="U57" s="20"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+    </row>
+    <row r="58" spans="1:25" ht="15.75">
+      <c r="A58" s="14"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="20"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="20"/>
+      <c r="V58" s="20"/>
+      <c r="W58" s="20"/>
+      <c r="X58" s="20"/>
+      <c r="Y58" s="20"/>
+    </row>
+    <row r="59" spans="1:25" ht="15.75">
+      <c r="A59" s="14"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="30"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="20"/>
+      <c r="S59" s="20"/>
+      <c r="T59" s="20"/>
+      <c r="U59" s="20"/>
+      <c r="V59" s="20"/>
+      <c r="W59" s="20"/>
+      <c r="X59" s="20"/>
+      <c r="Y59" s="20"/>
+    </row>
+    <row r="60" spans="1:25" ht="15.75">
+      <c r="A60" s="14"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="20"/>
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="20"/>
+      <c r="Y60" s="20"/>
+    </row>
+    <row r="61" spans="1:25" ht="15.75">
+      <c r="A61" s="14"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
+      <c r="V61" s="20"/>
+      <c r="W61" s="20"/>
+      <c r="X61" s="20"/>
+      <c r="Y61" s="20"/>
+    </row>
+    <row r="62" spans="1:25" ht="15.75">
+      <c r="A62" s="14"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="20"/>
+      <c r="T62" s="20"/>
+      <c r="U62" s="20"/>
+      <c r="V62" s="20"/>
+      <c r="W62" s="20"/>
+      <c r="X62" s="20"/>
+      <c r="Y62" s="20"/>
+    </row>
+    <row r="63" spans="1:25" ht="15.75">
+      <c r="A63" s="14"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="20"/>
+      <c r="R63" s="20"/>
+      <c r="S63" s="20"/>
+      <c r="T63" s="20"/>
+      <c r="U63" s="20"/>
+      <c r="V63" s="20"/>
+      <c r="W63" s="20"/>
+      <c r="X63" s="20"/>
+      <c r="Y63" s="20"/>
+    </row>
+    <row r="64" spans="1:25" ht="15.75">
+      <c r="A64" s="14"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="20"/>
+      <c r="S64" s="20"/>
+      <c r="T64" s="20"/>
+      <c r="U64" s="20"/>
+      <c r="V64" s="20"/>
+      <c r="W64" s="20"/>
+      <c r="X64" s="20"/>
+      <c r="Y64" s="20"/>
+    </row>
+    <row r="65" spans="1:25" ht="15.75">
+      <c r="A65" s="14"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="20"/>
+      <c r="R65" s="20"/>
+      <c r="S65" s="20"/>
+      <c r="T65" s="20"/>
+      <c r="U65" s="20"/>
+      <c r="V65" s="20"/>
+      <c r="W65" s="20"/>
+      <c r="X65" s="20"/>
+      <c r="Y65" s="20"/>
+    </row>
+    <row r="66" spans="1:25" ht="15.75">
+      <c r="A66" s="14"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="20"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="20"/>
+      <c r="X66" s="20"/>
+      <c r="Y66" s="20"/>
+    </row>
+    <row r="67" spans="1:25" ht="15.75">
+      <c r="A67" s="14"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="20"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="20"/>
+      <c r="O67" s="20"/>
+      <c r="P67" s="20"/>
+      <c r="Q67" s="20"/>
+      <c r="R67" s="20"/>
+      <c r="S67" s="20"/>
+      <c r="T67" s="20"/>
+      <c r="U67" s="20"/>
+      <c r="V67" s="20"/>
+      <c r="W67" s="20"/>
+      <c r="X67" s="20"/>
+      <c r="Y67" s="20"/>
+    </row>
+    <row r="68" spans="1:25" ht="15.75">
+      <c r="A68" s="14"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="20"/>
+      <c r="P68" s="20"/>
+      <c r="Q68" s="20"/>
+      <c r="R68" s="20"/>
+      <c r="S68" s="20"/>
+      <c r="T68" s="20"/>
+      <c r="U68" s="20"/>
+      <c r="V68" s="20"/>
+      <c r="W68" s="20"/>
+      <c r="X68" s="20"/>
+      <c r="Y68" s="20"/>
+    </row>
+    <row r="69" spans="1:25" ht="15.75">
+      <c r="A69" s="14"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="20"/>
+      <c r="N69" s="20"/>
+      <c r="O69" s="20"/>
+      <c r="P69" s="20"/>
+      <c r="Q69" s="20"/>
+      <c r="R69" s="20"/>
+      <c r="S69" s="20"/>
+      <c r="T69" s="20"/>
+      <c r="U69" s="20"/>
+      <c r="V69" s="20"/>
+      <c r="W69" s="20"/>
+      <c r="X69" s="20"/>
+      <c r="Y69" s="20"/>
+    </row>
+    <row r="70" spans="1:25" ht="15.75">
+      <c r="A70" s="14"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="20"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="20"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="20"/>
+      <c r="S70" s="20"/>
+      <c r="T70" s="20"/>
+      <c r="U70" s="20"/>
+      <c r="V70" s="20"/>
+      <c r="W70" s="20"/>
+      <c r="X70" s="20"/>
+      <c r="Y70" s="20"/>
+    </row>
+    <row r="71" spans="1:25" ht="15.75">
+      <c r="A71" s="24"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="20"/>
+      <c r="M71" s="20"/>
+      <c r="N71" s="20"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="20"/>
+      <c r="Q71" s="20"/>
+      <c r="R71" s="20"/>
+      <c r="S71" s="20"/>
+      <c r="T71" s="20"/>
+      <c r="U71" s="20"/>
+      <c r="V71" s="20"/>
+      <c r="W71" s="20"/>
+      <c r="X71" s="20"/>
+      <c r="Y71" s="20"/>
+    </row>
+    <row r="72" spans="1:25" ht="15.75">
+      <c r="A72" s="24"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="20"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="20"/>
+      <c r="Q72" s="20"/>
+      <c r="R72" s="20"/>
+      <c r="S72" s="20"/>
+      <c r="T72" s="20"/>
+      <c r="U72" s="20"/>
+      <c r="V72" s="20"/>
+      <c r="W72" s="20"/>
+      <c r="X72" s="20"/>
+      <c r="Y72" s="20"/>
+    </row>
+    <row r="73" spans="1:25" ht="15.75">
+      <c r="A73" s="24"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="20"/>
+      <c r="N73" s="20"/>
+      <c r="O73" s="20"/>
+      <c r="P73" s="20"/>
+      <c r="Q73" s="20"/>
+      <c r="R73" s="20"/>
+      <c r="S73" s="20"/>
+      <c r="T73" s="20"/>
+      <c r="U73" s="20"/>
+      <c r="V73" s="20"/>
+      <c r="W73" s="20"/>
+      <c r="X73" s="20"/>
+      <c r="Y73" s="20"/>
+    </row>
+    <row r="74" spans="1:25" ht="15.75"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F71:F73">
+      <formula1>"Pass, Fail, Pending, N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F7:F70">
+      <formula1>"Pass, Fail, Pending"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>